<commit_message>
Adiciona arquivos scripts DML e DQL
</commit_message>
<xml_diff>
--- a/manha/sprint1-bd-Gufi/modelagem/modelagem-Gufi.xlsx
+++ b/manha/sprint1-bd-Gufi/modelagem/modelagem-Gufi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adminlocal\Desktop\sprint1-bd-Gufi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adminlocal\Downloads\senai-dev-1s2020-alunos\sprint1-banco-de-dados\manha\sprint1-bd-Gufi\modelagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CBA4BC-D057-4C85-B71F-221A640F3DDA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A937C73E-5DE8-4EFD-AE13-156D650A60E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{2267D0F6-103C-4240-8365-61BC02ADDE06}"/>
   </bookViews>
@@ -386,49 +386,31 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -445,6 +427,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -764,7 +764,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -783,18 +783,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="31"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -810,16 +810,16 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="21" t="s">
         <v>15</v>
       </c>
       <c r="I2" s="1"/>
@@ -890,40 +890,40 @@
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="20"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="25" t="s">
         <v>49</v>
       </c>
       <c r="L7" s="1"/>
@@ -938,16 +938,16 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="29">
-        <v>1</v>
-      </c>
-      <c r="F8" s="29">
+      <c r="E8" s="24">
+        <v>1</v>
+      </c>
+      <c r="F8" s="24">
         <v>2</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="24">
         <v>2</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H8" s="30" t="s">
         <v>50</v>
       </c>
       <c r="I8" s="1"/>
@@ -965,16 +965,16 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="29">
+      <c r="E9" s="24">
         <v>2</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="24">
         <v>2</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="24">
         <v>3</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="30" t="s">
         <v>51</v>
       </c>
       <c r="I9" s="1"/>
@@ -992,16 +992,16 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="29">
+      <c r="E10" s="24">
         <v>3</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="24">
         <v>3</v>
       </c>
-      <c r="G10" s="29">
-        <v>1</v>
-      </c>
-      <c r="H10" s="36" t="s">
+      <c r="G10" s="24">
+        <v>1</v>
+      </c>
+      <c r="H10" s="30" t="s">
         <v>50</v>
       </c>
       <c r="I10" s="1"/>
@@ -1026,15 +1026,15 @@
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1043,25 +1043,25 @@
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="22" t="s">
+      <c r="B13" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="F13" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="20" t="s">
         <v>24</v>
       </c>
       <c r="H13" s="1"/>
@@ -1087,7 +1087,7 @@
       <c r="E14" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="27">
         <v>43867</v>
       </c>
       <c r="G14" s="7" t="s">
@@ -1116,7 +1116,7 @@
       <c r="E15" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="33">
+      <c r="F15" s="27">
         <v>43867</v>
       </c>
       <c r="G15" s="7" t="s">
@@ -1145,7 +1145,7 @@
       <c r="E16" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F16" s="27">
         <v>43867</v>
       </c>
       <c r="G16" s="7" t="s">
@@ -1174,15 +1174,15 @@
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1191,25 +1191,25 @@
       <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="34" t="s">
+      <c r="F19" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="27" t="s">
+      <c r="G19" s="23" t="s">
         <v>40</v>
       </c>
       <c r="H19" s="1"/>
@@ -1235,7 +1235,7 @@
       <c r="E20" s="11">
         <v>1</v>
       </c>
-      <c r="F20" s="35">
+      <c r="F20" s="29">
         <v>43868</v>
       </c>
       <c r="G20" s="10" t="s">
@@ -1264,7 +1264,7 @@
       <c r="E21" s="11">
         <v>0</v>
       </c>
-      <c r="F21" s="35">
+      <c r="F21" s="29">
         <v>43869</v>
       </c>
       <c r="G21" s="10" t="s">
@@ -1293,7 +1293,7 @@
       <c r="E22" s="11">
         <v>1</v>
       </c>
-      <c r="F22" s="35">
+      <c r="F22" s="29">
         <v>43870</v>
       </c>
       <c r="G22" s="10" t="s">

</xml_diff>